<commit_message>
Included sequential alignment in simulations
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUDA\Needleman-Wunsch\mini project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E471A349-AD54-47DC-A7DC-CB2B8F6F19E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E554AF4-3E42-48AB-99AA-E07078E95785}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E6E99AC1-04B7-4DC7-B5F4-9B69AE25DC52}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="SW" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Comparison!$A$3:$R$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Comparison!$A$3:$S$69</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="11">
   <si>
     <t>Alignment</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>SIMULATION RESULTS</t>
+  </si>
+  <si>
+    <t>seq(μs)</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +130,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -320,23 +329,91 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,18 +421,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,12 +435,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,22 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -428,6 +472,66 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,7 +646,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>nw(μs)</c:v>
+                  <c:v>seq(μs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -645,19 +749,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>190.63</c:v>
+                  <c:v>2479</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>330.88</c:v>
+                  <c:v>5477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>914.38</c:v>
+                  <c:v>12100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2753</c:v>
+                  <c:v>26735</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9990</c:v>
+                  <c:v>59167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,7 +781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>nm(μs)</c:v>
+                  <c:v>nw(μs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -780,19 +884,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>343.97</c:v>
+                  <c:v>190.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>814.7</c:v>
+                  <c:v>330.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3015</c:v>
+                  <c:v>914.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10041</c:v>
+                  <c:v>2753</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43413</c:v>
+                  <c:v>9990</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -812,7 +916,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pm(μs)</c:v>
+                  <c:v>nm(μs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -915,19 +1019,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>202.59</c:v>
+                  <c:v>343.97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>375.81</c:v>
+                  <c:v>814.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1112.4000000000001</c:v>
+                  <c:v>3015</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3547.3</c:v>
+                  <c:v>10041</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12998</c:v>
+                  <c:v>43413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,6 +1039,141 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A090-4A76-B571-E764629C7FC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$H$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pm(μs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Comparison!$D$16:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$H$16:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>202.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>375.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1112.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3547.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8989-4D63-ACAC-68D863E8C559}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10315,13 +10554,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>19051</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -10351,13 +10590,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
@@ -10387,13 +10626,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>600076</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -10950,339 +11189,361 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C4:L60"/>
+  <dimension ref="C4:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:12" ht="15" customHeight="1">
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="H4" s="32" t="s">
+    <row r="4" spans="3:13" ht="15" customHeight="1">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="I4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="20"/>
     </row>
-    <row r="5" spans="3:12" ht="15" customHeight="1">
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="31"/>
+    <row r="5" spans="3:13" ht="15" customHeight="1">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="20"/>
     </row>
-    <row r="6" spans="3:12" ht="15" customHeight="1">
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+    <row r="6" spans="3:13" ht="15" customHeight="1">
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
     </row>
-    <row r="7" spans="3:12" ht="18">
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+    <row r="7" spans="3:13" ht="18">
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="3:12" ht="18">
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+    <row r="8" spans="3:13" ht="18">
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
     </row>
-    <row r="13" spans="3:12" ht="15.75" thickBot="1"/>
-    <row r="14" spans="3:12" ht="15.75" thickBot="1">
-      <c r="D14" s="5" t="s">
+    <row r="13" spans="3:13" ht="15.75" thickBot="1"/>
+    <row r="14" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="3:12" ht="15.75" thickBot="1">
-      <c r="D15" s="11" t="s">
+    <row r="15" spans="3:13" ht="15.75" thickBot="1">
+      <c r="D15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="G15" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="3:12">
-      <c r="D16" s="8">
+    <row r="16" spans="3:13">
+      <c r="D16" s="4">
         <v>16</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="32">
+        <v>2479</v>
+      </c>
+      <c r="F16" s="10">
         <v>190.63</v>
       </c>
-      <c r="F16" s="16">
+      <c r="G16" s="36">
         <v>343.97</v>
       </c>
-      <c r="G16" s="17">
+      <c r="H16" s="40">
         <v>202.59</v>
       </c>
     </row>
-    <row r="17" spans="4:7">
-      <c r="D17" s="8">
+    <row r="17" spans="4:8">
+      <c r="D17" s="4">
         <v>32</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="32">
+        <v>5477</v>
+      </c>
+      <c r="F17" s="13">
         <v>330.88</v>
       </c>
-      <c r="F17" s="19">
+      <c r="G17" s="37">
         <v>814.7</v>
       </c>
-      <c r="G17" s="17">
+      <c r="H17" s="40">
         <v>375.81</v>
       </c>
     </row>
-    <row r="18" spans="4:7">
-      <c r="D18" s="8">
+    <row r="18" spans="4:8">
+      <c r="D18" s="4">
         <v>64</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="32">
+        <v>12100</v>
+      </c>
+      <c r="F18" s="13">
         <v>914.38</v>
       </c>
-      <c r="F18" s="19">
+      <c r="G18" s="37">
         <v>3015</v>
       </c>
-      <c r="G18" s="17">
+      <c r="H18" s="40">
         <v>1112.4000000000001</v>
       </c>
     </row>
-    <row r="19" spans="4:7">
-      <c r="D19" s="8">
+    <row r="19" spans="4:8">
+      <c r="D19" s="4">
         <v>128</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="32">
+        <v>26735</v>
+      </c>
+      <c r="F19" s="13">
         <v>2753</v>
       </c>
-      <c r="F19" s="19">
+      <c r="G19" s="37">
         <v>10041</v>
       </c>
-      <c r="G19" s="17">
+      <c r="H19" s="40">
         <v>3547.3</v>
       </c>
     </row>
-    <row r="20" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D20" s="9">
+    <row r="20" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D20" s="5">
         <v>256</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="33">
+        <v>59167</v>
+      </c>
+      <c r="F20" s="15">
         <v>9990</v>
       </c>
-      <c r="F20" s="21">
+      <c r="G20" s="38">
         <v>43413</v>
       </c>
-      <c r="G20" s="22">
+      <c r="H20" s="41">
         <v>12998</v>
       </c>
     </row>
-    <row r="33" spans="4:7" ht="15.75" thickBot="1"/>
-    <row r="34" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D34" s="23" t="s">
+    <row r="33" spans="4:8" ht="15.75" thickBot="1"/>
+    <row r="34" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D34" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="29"/>
     </row>
-    <row r="35" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D35" s="10" t="s">
+    <row r="35" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="4:7">
-      <c r="D36" s="10">
+    <row r="36" spans="4:8">
+      <c r="D36" s="6">
         <v>16</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="9">
         <v>1.32</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="10">
         <v>1.31</v>
       </c>
-      <c r="G36" s="27">
+      <c r="G36" s="17">
         <v>1.31</v>
       </c>
     </row>
-    <row r="37" spans="4:7">
-      <c r="D37" s="8">
+    <row r="37" spans="4:8">
+      <c r="D37" s="4">
         <v>32</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="12">
         <v>1.4</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="13">
         <v>1.31</v>
       </c>
-      <c r="G37" s="17">
+      <c r="G37" s="11">
         <v>1.34</v>
       </c>
     </row>
-    <row r="38" spans="4:7">
-      <c r="D38" s="8">
+    <row r="38" spans="4:8">
+      <c r="D38" s="4">
         <v>64</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="12">
         <v>1.4</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="13">
         <v>1.32</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="11">
         <v>1.34</v>
       </c>
     </row>
-    <row r="39" spans="4:7">
-      <c r="D39" s="8">
+    <row r="39" spans="4:8">
+      <c r="D39" s="4">
         <v>128</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="12">
         <v>1.36</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="13">
         <v>1.34</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="11">
         <v>1.47</v>
       </c>
     </row>
-    <row r="40" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D40" s="9">
+    <row r="40" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D40" s="5">
         <v>256</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="14">
         <v>1.55</v>
       </c>
-      <c r="F40" s="21">
+      <c r="F40" s="15">
         <v>1.53</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="16">
         <v>1.57</v>
       </c>
     </row>
-    <row r="53" spans="4:7" ht="15.75" thickBot="1"/>
-    <row r="54" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D54" s="23" t="s">
+    <row r="53" spans="4:8" ht="15.75" thickBot="1"/>
+    <row r="54" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D54" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="25"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="29"/>
     </row>
-    <row r="55" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D55" s="11" t="s">
+    <row r="55" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D55" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="28" t="s">
+      <c r="E55" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="4:7">
-      <c r="D56" s="8">
+    <row r="56" spans="4:8">
+      <c r="D56" s="4">
         <v>16</v>
       </c>
-      <c r="E56" s="18">
+      <c r="E56" s="12">
         <v>2.14</v>
       </c>
-      <c r="F56" s="19">
+      <c r="F56" s="13">
         <v>2.14</v>
       </c>
-      <c r="G56" s="17">
+      <c r="G56" s="11">
         <v>2.11</v>
       </c>
     </row>
-    <row r="57" spans="4:7">
-      <c r="D57" s="8">
+    <row r="57" spans="4:8">
+      <c r="D57" s="4">
         <v>32</v>
       </c>
-      <c r="E57" s="18">
+      <c r="E57" s="12">
         <v>2.23</v>
       </c>
-      <c r="F57" s="19">
+      <c r="F57" s="13">
         <v>2.17</v>
       </c>
-      <c r="G57" s="17">
+      <c r="G57" s="11">
         <v>2.14</v>
       </c>
     </row>
-    <row r="58" spans="4:7">
-      <c r="D58" s="8">
+    <row r="58" spans="4:8">
+      <c r="D58" s="4">
         <v>64</v>
       </c>
-      <c r="E58" s="18">
+      <c r="E58" s="12">
         <v>2.2400000000000002</v>
       </c>
-      <c r="F58" s="19">
+      <c r="F58" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G58" s="17">
+      <c r="G58" s="11">
         <v>2.17</v>
       </c>
     </row>
-    <row r="59" spans="4:7">
-      <c r="D59" s="8">
+    <row r="59" spans="4:8">
+      <c r="D59" s="4">
         <v>128</v>
       </c>
-      <c r="E59" s="18">
+      <c r="E59" s="12">
         <v>2.2799999999999998</v>
       </c>
-      <c r="F59" s="19">
+      <c r="F59" s="13">
         <v>2.36</v>
       </c>
-      <c r="G59" s="17">
+      <c r="G59" s="11">
         <v>2.17</v>
       </c>
     </row>
-    <row r="60" spans="4:7" ht="15.75" thickBot="1">
-      <c r="D60" s="9">
+    <row r="60" spans="4:8" ht="15.75" thickBot="1">
+      <c r="D60" s="5">
         <v>256</v>
       </c>
-      <c r="E60" s="20">
+      <c r="E60" s="14">
         <v>2.38</v>
       </c>
-      <c r="F60" s="21">
+      <c r="F60" s="15">
         <v>2.4900000000000002</v>
       </c>
-      <c r="G60" s="22">
+      <c r="G60" s="16">
         <v>2.33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="H4:K5"/>
-    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="I4:L5"/>
+    <mergeCell ref="D14:H14"/>
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="D54:G54"/>
   </mergeCells>
@@ -11310,18 +11571,18 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="4:11">
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="25"/>
+      <c r="G3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="25"/>
+      <c r="J3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">
@@ -11466,18 +11727,18 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="4:11">
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="25"/>
+      <c r="G3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="25"/>
+      <c r="J3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">

</xml_diff>